<commit_message>
README update, streams step 8 complete, contribute page added
</commit_message>
<xml_diff>
--- a/AspenStreams03122020.xlsx
+++ b/AspenStreams03122020.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/roeelandesman/Desktop/SP/src/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C5F4BE8-ED23-D846-9FF6-482187AA488D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{385909E8-E21B-174A-9863-919A6E10AEFB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="12940" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="19040" windowHeight="12180" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Aspen Data Tables" sheetId="1" r:id="rId1"/>
@@ -664,7 +664,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -672,7 +672,6 @@
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -959,162 +958,160 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A2:CY135"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F28" sqref="F28"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="22.6640625" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10" style="3" bestFit="1" customWidth="1"/>
-    <col min="3" max="12" width="12.1640625" style="3" bestFit="1" customWidth="1"/>
-    <col min="13" max="14" width="12" style="3" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="12.1640625" style="3" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="12" style="3" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="10" style="3" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="12.1640625" style="3" bestFit="1" customWidth="1"/>
-    <col min="19" max="21" width="12" style="3" bestFit="1" customWidth="1"/>
-    <col min="22" max="24" width="12.1640625" style="3" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="12" style="3" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="12.1640625" style="3" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="12" style="3" bestFit="1" customWidth="1"/>
-    <col min="28" max="37" width="12.1640625" style="3" bestFit="1" customWidth="1"/>
-    <col min="38" max="39" width="12" style="3" bestFit="1" customWidth="1"/>
-    <col min="40" max="40" width="12.1640625" style="3" bestFit="1" customWidth="1"/>
-    <col min="41" max="45" width="12" style="3" bestFit="1" customWidth="1"/>
-    <col min="46" max="46" width="12.1640625" style="3" bestFit="1" customWidth="1"/>
-    <col min="47" max="51" width="12" style="3" bestFit="1" customWidth="1"/>
-    <col min="52" max="52" width="12.1640625" style="3" bestFit="1" customWidth="1"/>
-    <col min="53" max="53" width="12" style="3" bestFit="1" customWidth="1"/>
-    <col min="54" max="54" width="12.1640625" style="3" bestFit="1" customWidth="1"/>
-    <col min="55" max="57" width="12" style="3" bestFit="1" customWidth="1"/>
-    <col min="58" max="58" width="12.1640625" style="3" bestFit="1" customWidth="1"/>
-    <col min="59" max="59" width="12" style="3" bestFit="1" customWidth="1"/>
-    <col min="60" max="63" width="12.1640625" style="3" bestFit="1" customWidth="1"/>
-    <col min="64" max="64" width="12" style="3" bestFit="1" customWidth="1"/>
-    <col min="65" max="70" width="12.1640625" style="3" bestFit="1" customWidth="1"/>
-    <col min="71" max="71" width="12" style="3" bestFit="1" customWidth="1"/>
-    <col min="72" max="77" width="12.1640625" style="3" bestFit="1" customWidth="1"/>
-    <col min="78" max="78" width="12" style="3" bestFit="1" customWidth="1"/>
-    <col min="79" max="81" width="12.1640625" style="3" bestFit="1" customWidth="1"/>
-    <col min="82" max="82" width="9.33203125" style="3" bestFit="1" customWidth="1"/>
-    <col min="83" max="93" width="12" style="3" bestFit="1" customWidth="1"/>
-    <col min="95" max="95" width="13.1640625" style="3" bestFit="1" customWidth="1"/>
-    <col min="96" max="96" width="11" style="3" bestFit="1" customWidth="1"/>
-    <col min="97" max="97" width="11.6640625" style="3" bestFit="1" customWidth="1"/>
-    <col min="98" max="98" width="11" style="3" bestFit="1" customWidth="1"/>
-    <col min="99" max="99" width="11.6640625" style="3" bestFit="1" customWidth="1"/>
-    <col min="100" max="101" width="11" style="3" bestFit="1" customWidth="1"/>
-    <col min="102" max="103" width="11.6640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="22.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10" bestFit="1" customWidth="1"/>
+    <col min="3" max="12" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="13" max="14" width="12" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="12" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="10" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="19" max="21" width="12" bestFit="1" customWidth="1"/>
+    <col min="22" max="24" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="12" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="12" bestFit="1" customWidth="1"/>
+    <col min="28" max="37" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="38" max="39" width="12" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="41" max="45" width="12" bestFit="1" customWidth="1"/>
+    <col min="46" max="46" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="47" max="51" width="12" bestFit="1" customWidth="1"/>
+    <col min="52" max="52" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="53" max="53" width="12" bestFit="1" customWidth="1"/>
+    <col min="54" max="54" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="55" max="57" width="12" bestFit="1" customWidth="1"/>
+    <col min="58" max="58" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="59" max="59" width="12" bestFit="1" customWidth="1"/>
+    <col min="60" max="63" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="64" max="64" width="12" bestFit="1" customWidth="1"/>
+    <col min="65" max="70" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="71" max="71" width="12" bestFit="1" customWidth="1"/>
+    <col min="72" max="77" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="78" max="78" width="12" bestFit="1" customWidth="1"/>
+    <col min="79" max="81" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="82" max="82" width="9.33203125" bestFit="1" customWidth="1"/>
+    <col min="83" max="93" width="12" bestFit="1" customWidth="1"/>
+    <col min="95" max="95" width="13.1640625" bestFit="1" customWidth="1"/>
+    <col min="96" max="96" width="11" bestFit="1" customWidth="1"/>
+    <col min="97" max="97" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="98" max="98" width="11" bestFit="1" customWidth="1"/>
+    <col min="99" max="99" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="100" max="101" width="11" bestFit="1" customWidth="1"/>
+    <col min="102" max="103" width="11.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:103" x14ac:dyDescent="0.2">
-      <c r="A2" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="5"/>
-      <c r="C2" s="5"/>
-      <c r="D2" s="5"/>
-      <c r="E2" s="5"/>
-      <c r="F2" s="5"/>
-      <c r="G2" s="5"/>
-      <c r="H2" s="5"/>
-      <c r="I2" s="5"/>
-      <c r="J2" s="5"/>
-      <c r="K2" s="5"/>
-      <c r="L2" s="5"/>
-      <c r="M2" s="5"/>
-      <c r="N2" s="5"/>
-      <c r="O2" s="5"/>
-      <c r="P2" s="5"/>
-      <c r="Q2" s="5"/>
-      <c r="R2" s="5"/>
-      <c r="S2" s="5"/>
-      <c r="T2" s="5"/>
-      <c r="U2" s="5"/>
-      <c r="V2" s="5"/>
-      <c r="W2" s="5"/>
-      <c r="X2" s="5"/>
-      <c r="Y2" s="5"/>
-      <c r="Z2" s="5"/>
-      <c r="AA2" s="5"/>
-      <c r="AB2" s="5"/>
-      <c r="AC2" s="5"/>
-      <c r="AD2" s="5"/>
-      <c r="AE2" s="5"/>
-      <c r="AF2" s="5"/>
-      <c r="AG2" s="5"/>
-      <c r="AH2" s="5"/>
-      <c r="AI2" s="5"/>
-      <c r="AJ2" s="5"/>
-      <c r="AK2" s="5"/>
-      <c r="AL2" s="5"/>
-      <c r="AM2" s="5"/>
-      <c r="AN2" s="5"/>
-      <c r="AO2" s="5"/>
-      <c r="AP2" s="5"/>
-      <c r="AQ2" s="5"/>
-      <c r="AR2" s="5"/>
-      <c r="AS2" s="5"/>
-      <c r="AT2" s="5"/>
-      <c r="AU2" s="5"/>
-      <c r="AV2" s="5"/>
-      <c r="AW2" s="5"/>
-      <c r="AX2" s="5"/>
-      <c r="AY2" s="5"/>
-      <c r="AZ2" s="5"/>
-      <c r="BA2" s="5"/>
-      <c r="BB2" s="5"/>
-      <c r="BC2" s="5"/>
-      <c r="BD2" s="5"/>
-      <c r="BE2" s="5"/>
-      <c r="BF2" s="5"/>
-      <c r="BG2" s="5"/>
-      <c r="BH2" s="5"/>
-      <c r="BI2" s="5"/>
-      <c r="BJ2" s="5"/>
-      <c r="BK2" s="5"/>
-      <c r="BL2" s="5"/>
-      <c r="BM2" s="5"/>
-      <c r="BN2" s="5"/>
-      <c r="BO2" s="5"/>
-      <c r="BP2" s="5"/>
-      <c r="BQ2" s="5"/>
-      <c r="BR2" s="5"/>
-      <c r="BS2" s="5"/>
-      <c r="BT2" s="5"/>
-      <c r="BU2" s="5"/>
-      <c r="BV2" s="5"/>
-      <c r="BW2" s="5"/>
-      <c r="BX2" s="5"/>
-      <c r="BY2" s="5"/>
-      <c r="BZ2" s="5"/>
-      <c r="CA2" s="5"/>
-      <c r="CB2" s="5"/>
-      <c r="CC2" s="5"/>
-      <c r="CD2" s="5"/>
-      <c r="CE2" s="5"/>
-      <c r="CF2" s="5"/>
-      <c r="CG2" s="5"/>
-      <c r="CH2" s="5"/>
-      <c r="CI2" s="5"/>
-      <c r="CJ2" s="5"/>
-      <c r="CK2" s="5"/>
-      <c r="CL2" s="5"/>
-      <c r="CM2" s="5"/>
-      <c r="CN2" s="5"/>
-      <c r="CO2" s="5"/>
-      <c r="CQ2" s="4" t="s">
+      <c r="A2" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="4"/>
+      <c r="C2" s="4"/>
+      <c r="D2" s="4"/>
+      <c r="E2" s="4"/>
+      <c r="F2" s="4"/>
+      <c r="G2" s="4"/>
+      <c r="H2" s="4"/>
+      <c r="I2" s="4"/>
+      <c r="J2" s="4"/>
+      <c r="K2" s="4"/>
+      <c r="L2" s="4"/>
+      <c r="M2" s="4"/>
+      <c r="N2" s="4"/>
+      <c r="O2" s="4"/>
+      <c r="P2" s="4"/>
+      <c r="Q2" s="4"/>
+      <c r="R2" s="4"/>
+      <c r="S2" s="4"/>
+      <c r="T2" s="4"/>
+      <c r="U2" s="4"/>
+      <c r="V2" s="4"/>
+      <c r="W2" s="4"/>
+      <c r="X2" s="4"/>
+      <c r="Y2" s="4"/>
+      <c r="Z2" s="4"/>
+      <c r="AA2" s="4"/>
+      <c r="AB2" s="4"/>
+      <c r="AC2" s="4"/>
+      <c r="AD2" s="4"/>
+      <c r="AE2" s="4"/>
+      <c r="AF2" s="4"/>
+      <c r="AG2" s="4"/>
+      <c r="AH2" s="4"/>
+      <c r="AI2" s="4"/>
+      <c r="AJ2" s="4"/>
+      <c r="AK2" s="4"/>
+      <c r="AL2" s="4"/>
+      <c r="AM2" s="4"/>
+      <c r="AN2" s="4"/>
+      <c r="AO2" s="4"/>
+      <c r="AP2" s="4"/>
+      <c r="AQ2" s="4"/>
+      <c r="AR2" s="4"/>
+      <c r="AS2" s="4"/>
+      <c r="AT2" s="4"/>
+      <c r="AU2" s="4"/>
+      <c r="AV2" s="4"/>
+      <c r="AW2" s="4"/>
+      <c r="AX2" s="4"/>
+      <c r="AY2" s="4"/>
+      <c r="AZ2" s="4"/>
+      <c r="BA2" s="4"/>
+      <c r="BB2" s="4"/>
+      <c r="BC2" s="4"/>
+      <c r="BD2" s="4"/>
+      <c r="BE2" s="4"/>
+      <c r="BF2" s="4"/>
+      <c r="BG2" s="4"/>
+      <c r="BH2" s="4"/>
+      <c r="BI2" s="4"/>
+      <c r="BJ2" s="4"/>
+      <c r="BK2" s="4"/>
+      <c r="BL2" s="4"/>
+      <c r="BM2" s="4"/>
+      <c r="BN2" s="4"/>
+      <c r="BO2" s="4"/>
+      <c r="BP2" s="4"/>
+      <c r="BQ2" s="4"/>
+      <c r="BR2" s="4"/>
+      <c r="BS2" s="4"/>
+      <c r="BT2" s="4"/>
+      <c r="BU2" s="4"/>
+      <c r="BV2" s="4"/>
+      <c r="BW2" s="4"/>
+      <c r="BX2" s="4"/>
+      <c r="BY2" s="4"/>
+      <c r="BZ2" s="4"/>
+      <c r="CA2" s="4"/>
+      <c r="CB2" s="4"/>
+      <c r="CC2" s="4"/>
+      <c r="CD2" s="4"/>
+      <c r="CE2" s="4"/>
+      <c r="CF2" s="4"/>
+      <c r="CG2" s="4"/>
+      <c r="CH2" s="4"/>
+      <c r="CI2" s="4"/>
+      <c r="CJ2" s="4"/>
+      <c r="CK2" s="4"/>
+      <c r="CL2" s="4"/>
+      <c r="CM2" s="4"/>
+      <c r="CN2" s="4"/>
+      <c r="CO2" s="4"/>
+      <c r="CQ2" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="CR2" s="5"/>
-      <c r="CS2" s="5"/>
-      <c r="CT2" s="5"/>
-      <c r="CU2" s="5"/>
-      <c r="CV2" s="5"/>
-      <c r="CW2" s="5"/>
-      <c r="CX2" s="5"/>
-      <c r="CY2" s="5"/>
+      <c r="CR2" s="4"/>
+      <c r="CS2" s="4"/>
+      <c r="CT2" s="4"/>
+      <c r="CU2" s="4"/>
+      <c r="CV2" s="4"/>
+      <c r="CW2" s="4"/>
+      <c r="CX2" s="4"/>
+      <c r="CY2" s="4"/>
     </row>
     <row r="3" spans="1:103" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
@@ -30473,6 +30470,5 @@
     <mergeCell ref="CQ2:CY2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>